<commit_message>
[minor] Improvements and fixes
</commit_message>
<xml_diff>
--- a/timecard.xlsx
+++ b/timecard.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Python35-32\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vn0w5m5/Desktop/Timecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4C7F24-B922-3347-A731-698947FBE01F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12435"/>
+    <workbookView xWindow="13280" yWindow="460" windowWidth="25120" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Day</t>
   </si>
@@ -56,22 +57,34 @@
     <t>Time Out</t>
   </si>
   <si>
-    <t>12:00 PM</t>
-  </si>
-  <si>
-    <t>7:30 AM</t>
-  </si>
-  <si>
-    <t>12:30 PM</t>
-  </si>
-  <si>
-    <t>4:00 PM</t>
+    <t>10:00 AM</t>
+  </si>
+  <si>
+    <t>9:00 AM</t>
+  </si>
+  <si>
+    <t>6:00 PM</t>
+  </si>
+  <si>
+    <t>5:00 PM</t>
+  </si>
+  <si>
+    <t>10:00AM</t>
+  </si>
+  <si>
+    <t>6:00PM</t>
+  </si>
+  <si>
+    <t>Sat</t>
+  </si>
+  <si>
+    <t>Sun</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -88,7 +101,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,6 +136,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -159,7 +178,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -174,6 +193,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -459,119 +479,105 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F5"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="D2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>10</v>
-      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="D5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
     </row>

</xml_diff>